<commit_message>
Fix PO import vendor price
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Zalo Received Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8D40A-DF91-4DF0-AEAB-F3D3BCAFC39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
@@ -22,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{56C6A7C2-98CB-45BE-99CC-C0709C07AD5F}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{FFCD09BB-7986-4C81-ACAE-594C66B213F2}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{202938D7-88EA-4A28-BAC5-37D9B2AE089A}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,12 +109,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3E7DBBB6-6DA6-43F9-BB77-319144B7DFB2}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B3441D31-85C4-4ADE-BED0-372B79909630}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{23B017A6-16A1-47E0-8B43-CB09FE54DB50}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,12 +193,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2CF4CA4D-C97D-4881-A863-B3C3F5E9D7FC}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B0289F6E-FFDC-429D-B65D-6245DFD5729F}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -247,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{45C6E384-E8BF-49A4-9DBB-3E9EE9EE607F}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -353,7 +352,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -363,7 +362,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -378,7 +377,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -388,7 +387,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -403,7 +402,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -413,7 +412,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -428,7 +427,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -438,7 +437,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -456,7 +455,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -466,7 +465,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -481,7 +480,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -491,7 +490,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -506,7 +505,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -516,7 +515,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -531,7 +530,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -541,7 +540,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -556,7 +555,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -566,7 +565,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -581,7 +580,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -591,7 +590,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -612,7 +611,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -622,7 +621,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -638,7 +637,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -648,7 +647,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -663,7 +662,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -673,7 +672,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -688,7 +687,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -698,7 +697,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -706,14 +705,45 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Chi tiết đơn hàng / Giá của nhà cung cấp (</t>
+    <t>Chi tiết đơn hàng  / Thành tiền VND của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế nhập khẩu</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / Thuế nhập khẩu của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế tiêu thụ đặc biệt</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  /  Thuế TTĐB của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế GTGT</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / Thuế GTGT của sản phẩm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi phí / Tiền tệ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -723,7 +753,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -731,45 +761,71 @@
     </r>
   </si>
   <si>
-    <t>Chi tiết đơn hàng  / Thành tiền VND của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế nhập khẩu</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / Thuế nhập khẩu của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế tiêu thụ đặc biệt</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  /  Thuế TTĐB của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế GTGT</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / Thuế GTGT của sản phẩm</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi phí / Tiền tệ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
+    <t>Zoey</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Nhập khẩu quần áo</t>
+  </si>
+  <si>
+    <t>1551_TP001</t>
+  </si>
+  <si>
+    <t>POLO2023</t>
+  </si>
+  <si>
+    <t>PR204</t>
+  </si>
+  <si>
+    <t>1562_CPHH</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Số lượng (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>(</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -779,7 +835,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -787,35 +843,18 @@
     </r>
   </si>
   <si>
-    <t>Zoey</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Nhập khẩu quần áo</t>
-  </si>
-  <si>
-    <t>1551_TP001</t>
-  </si>
-  <si>
-    <t>POLO2023</t>
-  </si>
-  <si>
-    <t>PR204</t>
-  </si>
-  <si>
-    <t>1562_CPHH</t>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết đơn hàng / Số lượng (</t>
-    </r>
-    <r>
-      <rPr>
+    <t>622_NCNB</t>
+  </si>
+  <si>
+    <r>
+      <t>Tỷ giá (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -825,7 +864,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -833,105 +872,43 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>622_NCNB</t>
-  </si>
-  <si>
-    <r>
-      <t>Tỷ giá (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
+    <t>Chi tiết đơn hàng / Giá của nhà cung cấp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -953,21 +930,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -996,7 +973,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -1060,7 +1037,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1069,29 +1046,29 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Tiền tệ" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1423,55 +1400,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.19921875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="30.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.796875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.3984375" style="1" customWidth="1"/>
-    <col min="22" max="22" width="26.8984375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="30.8984375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="32.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="26.85546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="30.85546875" style="6" customWidth="1"/>
     <col min="24" max="24" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.59765625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="24.19921875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="22.09765625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="23.09765625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.09765625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="25.8984375" style="1" customWidth="1"/>
-    <col min="38" max="38" width="20.09765625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.59765625" style="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.8984375" style="1"/>
+    <col min="32" max="32" width="22.5703125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="24.140625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="22.140625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="23.140625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="25.85546875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="20.140625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.5703125" style="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="17" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,7 +1504,7 @@
         <v>30</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="S1" s="9" t="s">
         <v>31</v>
@@ -1554,7 +1531,7 @@
         <v>34</v>
       </c>
       <c r="AA1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AB1" s="13" t="s">
         <v>18</v>
@@ -1571,13 +1548,13 @@
     </row>
     <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1604,10 +1581,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="N2" s="1" t="b">
         <v>0</v>
@@ -1631,22 +1608,22 @@
         <v>2</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="X2" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y2" s="1">
         <v>1</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AB2" s="1">
         <v>23960</v>
@@ -1672,42 +1649,42 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E94CD2-F881-4057-99CD-CBE2B9D96557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.3984375" customWidth="1"/>
-    <col min="3" max="3" width="10.3984375" customWidth="1"/>
-    <col min="4" max="4" width="15.8984375" customWidth="1"/>
-    <col min="5" max="5" width="20.796875" customWidth="1"/>
-    <col min="6" max="6" width="13.796875" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="15.796875" customWidth="1"/>
-    <col min="10" max="10" width="15.09765625" customWidth="1"/>
-    <col min="12" max="12" width="31.09765625" customWidth="1"/>
-    <col min="13" max="13" width="26.296875" customWidth="1"/>
-    <col min="14" max="14" width="33.5" customWidth="1"/>
-    <col min="15" max="15" width="31.09765625" customWidth="1"/>
+    <col min="1" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="31.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" customWidth="1"/>
     <col min="16" max="16" width="35" customWidth="1"/>
-    <col min="17" max="17" width="35.69921875" customWidth="1"/>
-    <col min="18" max="18" width="30.69921875" customWidth="1"/>
-    <col min="19" max="19" width="27.69921875" customWidth="1"/>
+    <col min="17" max="17" width="35.7109375" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" customWidth="1"/>
+    <col min="19" max="19" width="27.7109375" customWidth="1"/>
     <col min="20" max="20" width="27" customWidth="1"/>
-    <col min="21" max="21" width="27.8984375" customWidth="1"/>
-    <col min="22" max="22" width="29.09765625" customWidth="1"/>
-    <col min="23" max="23" width="34.59765625" customWidth="1"/>
-    <col min="24" max="24" width="29.5" customWidth="1"/>
-    <col min="25" max="25" width="19.8984375" customWidth="1"/>
-    <col min="26" max="26" width="15.5" customWidth="1"/>
-    <col min="27" max="27" width="14.59765625" customWidth="1"/>
-    <col min="28" max="28" width="25.8984375" customWidth="1"/>
-    <col min="29" max="29" width="22.5" customWidth="1"/>
-    <col min="30" max="30" width="25.19921875" customWidth="1"/>
+    <col min="21" max="21" width="27.85546875" customWidth="1"/>
+    <col min="22" max="22" width="29.140625" customWidth="1"/>
+    <col min="23" max="23" width="34.5703125" customWidth="1"/>
+    <col min="24" max="24" width="29.42578125" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" customWidth="1"/>
+    <col min="28" max="28" width="25.85546875" customWidth="1"/>
+    <col min="29" max="29" width="22.42578125" customWidth="1"/>
+    <col min="30" max="30" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1751,13 +1728,13 @@
         <v>9</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>29</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>10</v>
@@ -1783,13 +1760,13 @@
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1816,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -1837,7 +1814,7 @@
         <v>6</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
@@ -1857,49 +1834,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B4FA9B-1F49-4C23-93F7-CC7DAC82722D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.19921875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.09765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.69921875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="28" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.8984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="42" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="42.296875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="36.796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="39.19921875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.09765625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.8984375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
@@ -1910,7 +1887,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>24</v>
@@ -1940,13 +1917,13 @@
         <v>9</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>29</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>10</v>
@@ -1970,31 +1947,31 @@
         <v>33</v>
       </c>
       <c r="X1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="16" t="s">
+      <c r="Z1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="16" t="s">
+      <c r="AB1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="16" t="s">
+      <c r="AC1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="16" t="s">
+      <c r="AD1" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="AD1" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="AE1" s="13" t="s">
         <v>34</v>
       </c>
       <c r="AF1" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AG1" s="13" t="s">
         <v>18</v>
@@ -2011,13 +1988,13 @@
     </row>
     <row r="2" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2044,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -2068,7 +2045,7 @@
         <v>6</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
@@ -2213,18 +2190,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2246,6 +2223,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2259,12 +2244,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix header template import
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D5AFF4-CE44-4387-86AC-9ABD5446E13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
@@ -22,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{56C6A7C2-98CB-45BE-99CC-C0709C07AD5F}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{FFCD09BB-7986-4C81-ACAE-594C66B213F2}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{202938D7-88EA-4A28-BAC5-37D9B2AE089A}">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,12 +109,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3E7DBBB6-6DA6-43F9-BB77-319144B7DFB2}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -139,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B3441D31-85C4-4ADE-BED0-372B79909630}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{23B017A6-16A1-47E0-8B43-CB09FE54DB50}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,13 +193,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>DELL</author>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{9B1A416B-8E22-4CF8-A3C9-324CB69C64A5}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{ECF6FC0F-5F86-4595-BCB2-ACBB11F68CBA}">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +243,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{7D929D66-DD2C-45AE-8071-6B1E367EBEA7}">
+    <comment ref="L1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{7107DDE2-34FF-4DC3-8869-2D471E91904E}">
+    <comment ref="M1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -296,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{9FCDEF59-4CD2-4C1C-9DD8-B2B04A88FEA2}">
+    <comment ref="P1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -322,7 +321,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{66C60A60-F8D8-42A6-9E9C-A1B33679AFA9}">
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -349,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
   <si>
     <t>Note</t>
   </si>
@@ -994,9 +993,6 @@
     </r>
   </si>
   <si>
-    <t>Chi phí / Tiền tệ</t>
-  </si>
-  <si>
     <t>3000000004</t>
   </si>
   <si>
@@ -1004,12 +1000,55 @@
   </si>
   <si>
     <t>P002648</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Tỷ lệ quy đổi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Mã Sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tiền tệ</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tỷ giá</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tổng tiền ngoại tệ̣</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Thành tiền VND</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Chi phí trước thuế</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
@@ -1540,7 +1579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1789,7 +1828,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E94CD2-F881-4057-99CD-CBE2B9D96557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1974,11 +2013,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B4FA9B-1F49-4C23-93F7-CC7DAC82722D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2120,7 @@
         <v>38</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="T1" s="9" t="s">
         <v>39</v>
@@ -2102,33 +2141,33 @@
         <v>32</v>
       </c>
       <c r="Z1" s="13" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="AA1" s="13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="AD1" s="13" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="AE1" s="13" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2150,7 +2189,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="1" t="b">
         <v>0</v>
@@ -2230,12 +2269,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x01010015570558A7E4E34C9FC908F8AA8CCE03" ma:contentTypeVersion="2" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="b5e9dccfa7c94a2dc6af17131503e849">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6a70de89-a9ee-4e6f-a4d0-6241823bbbed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="12f1dcc1fa3bdb4d5e8deb26a304abcf" ns2:_="">
     <xsd:import namespace="6a70de89-a9ee-4e6f-a4d0-6241823bbbed"/>
@@ -2367,6 +2400,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
   <ds:schemaRefs>
@@ -2376,22 +2415,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6a70de89-a9ee-4e6f-a4d0-6241823bbbed"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD4940E0-21AB-4BF6-89A9-5D6EDC45D85E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2407,4 +2430,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6a70de89-a9ee-4e6f-a4d0-6241823bbbed"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix template lien cty
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
@@ -26,32 +26,6 @@
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="163"/>
-          </rPr>
-          <t>Nguyễn Văn Quyết (DU01 PTPM):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="163"/>
-          </rPr>
-          <t xml:space="preserve">
-1/0</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -78,7 +52,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>Nguyễn Văn Quyết (DU01 PTPM):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+1/0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -348,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
   <si>
     <t>Note</t>
   </si>
@@ -404,18 +404,6 @@
     <t>Chiếc</t>
   </si>
   <si>
-    <t>Chi phí / Tỷ giá</t>
-  </si>
-  <si>
-    <t>Chi phí / Tổng tiền ngoại tệ̣</t>
-  </si>
-  <si>
-    <t>Chi phí / Chi phí trước thuế</t>
-  </si>
-  <si>
-    <t>Chi phí / Thành tiền VND</t>
-  </si>
-  <si>
     <r>
       <t>Nhà cung cấp (</t>
     </r>
@@ -595,7 +583,7 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết đơn hàng / Số lượng quy đổi (</t>
+      <t>Chi tiết đơn hàng / Địa điểm kho (</t>
     </r>
     <r>
       <rPr>
@@ -620,7 +608,7 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết đơn hàng / Địa điểm kho (</t>
+      <t>Chi tiết đơn hàng / Ngày nhận (</t>
     </r>
     <r>
       <rPr>
@@ -644,8 +632,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Chi tiết đơn hàng / Ngày nhận (</t>
+    <t>Chi tiết đơn hàng / STT Dòng YCMH</t>
+  </si>
+  <si>
+    <r>
+      <t>Tiền tệ (</t>
     </r>
     <r>
       <rPr>
@@ -663,20 +654,15 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
-    <t>Chi tiết đơn hàng / STT Dòng YCMH</t>
-  </si>
-  <si>
-    <t>Chi phí / Mã Sản phẩm</t>
-  </si>
-  <si>
-    <r>
-      <t>Tiền tệ (</t>
+    <r>
+      <t>Tỷ giá (</t>
     </r>
     <r>
       <rPr>
@@ -694,15 +680,39 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hạn xử lý  (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Tỷ giá (</t>
+      <t xml:space="preserve">Chi tiết đơn hàng / Đơn vị mua </t>
     </r>
     <r>
       <rPr>
@@ -713,6 +723,31 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
+      <t>(*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Giá của nhà cung cấp (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>*</t>
     </r>
     <r>
@@ -726,8 +761,29 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Hạn xử lý  (</t>
+    <t>Zoey</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Nhập khẩu quần áo</t>
+  </si>
+  <si>
+    <t>1551_TP001</t>
+  </si>
+  <si>
+    <t>POLO2023</t>
+  </si>
+  <si>
+    <t>PR204</t>
+  </si>
+  <si>
+    <t>1562_CPHH</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Số lượng (</t>
     </r>
     <r>
       <rPr>
@@ -752,7 +808,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn vị mua </t>
+      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
     </r>
     <r>
       <rPr>
@@ -763,7 +830,7 @@
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(*</t>
+      <t>*</t>
     </r>
     <r>
       <rPr>
@@ -776,8 +843,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Chi tiết đơn hàng / Giá của nhà cung cấp (</t>
+    <t>622_NCNB</t>
+  </si>
+  <si>
+    <r>
+      <t>Kho nguồn (</t>
     </r>
     <r>
       <rPr>
@@ -785,6 +855,87 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kho nhận (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tài liệu gốc (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>3000000004</t>
+  </si>
+  <si>
+    <t>VND</t>
+  </si>
+  <si>
+    <t>P002648</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Tỷ lệ quy đổi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
@@ -801,8 +952,26 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Chi phí / Tiền tệ </t>
+    <t>Chi phí ước tính / Mã Sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tiền tệ</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tỷ giá</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tổng tiền ngoại tệ̣</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Thành tiền VND</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Chi phí trước thuế</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi phí ước tính / Tiền tệ </t>
     </r>
     <r>
       <rPr>
@@ -836,213 +1005,7 @@
     </r>
   </si>
   <si>
-    <t>Zoey</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Nhập khẩu quần áo</t>
-  </si>
-  <si>
-    <t>1551_TP001</t>
-  </si>
-  <si>
-    <t>POLO2023</t>
-  </si>
-  <si>
-    <t>PR204</t>
-  </si>
-  <si>
-    <t>1562_CPHH</t>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết đơn hàng / Số lượng (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>622_NCNB</t>
-  </si>
-  <si>
-    <r>
-      <t>Kho nguồn (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Kho nhận (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Tài liệu gốc (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>3000000004</t>
-  </si>
-  <si>
-    <t>VND</t>
-  </si>
-  <si>
-    <t>P002648</t>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết đơn hàng / Tỷ lệ quy đổi (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Mã Sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Tiền tệ</t>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Tỷ giá</t>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Tổng tiền ngoại tệ̣</t>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Thành tiền VND</t>
-  </si>
-  <si>
-    <t>Chi phí ước tính / Chi phí trước thuế</t>
+    <t>Kho nguồn</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1234,6 +1197,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1580,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,144 +1560,148 @@
     <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="32.42578125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="30.85546875" style="6" customWidth="1"/>
-    <col min="24" max="24" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.5703125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="24.140625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="22.140625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="23.140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="25.85546875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="20.140625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.5703125" style="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.85546875" style="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="32.42578125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="26.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="30.85546875" style="6" customWidth="1"/>
+    <col min="25" max="25" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.5703125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="24.140625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="22.140625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="23.140625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" style="1" customWidth="1"/>
+    <col min="38" max="38" width="25.85546875" style="1" customWidth="1"/>
+    <col min="39" max="39" width="20.140625" style="1" customWidth="1"/>
+    <col min="40" max="40" width="22.5703125" style="1" customWidth="1"/>
+    <col min="41" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="15" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="15" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1753,71 +1721,74 @@
       <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="b">
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="K2" s="1" t="b">
+      <c r="L2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="1" t="b">
+        <v>36</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>20</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="12">
+      <c r="R2" s="12">
         <v>1</v>
       </c>
-      <c r="R2" s="1">
+      <c r="S2" s="1">
         <v>10</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>2</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="W2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z2" s="1">
         <v>1</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="AA2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC2" s="1">
         <v>23960</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>50</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>1198000</v>
       </c>
-      <c r="AE2" s="1" t="b">
+      <c r="AF2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
     </row>
   </sheetData>
@@ -1832,7 +1803,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,28 +1839,28 @@
   <sheetData>
     <row r="1" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
@@ -1901,19 +1872,19 @@
         <v>4</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>10</v>
@@ -1928,24 +1899,24 @@
         <v>14</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>15</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1972,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -1993,7 +1964,7 @@
         <v>6</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
@@ -2016,8 +1987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,37 +2037,37 @@
   <sheetData>
     <row r="1" spans="1:31" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>8</v>
@@ -2108,25 +2079,25 @@
         <v>4</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="S1" s="11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="T1" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>10</v>
@@ -2138,36 +2109,36 @@
         <v>12</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Z1" s="13" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="AD1" s="13" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="AE1" s="13" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2189,7 +2160,7 @@
         <v>16</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="L2" s="1" t="b">
         <v>0</v>
@@ -2198,10 +2169,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="P2" s="1" t="b">
         <v>0</v>
@@ -2222,17 +2193,17 @@
         <v>16</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AB2" s="1">
         <v>23960</v>

</xml_diff>

<commit_message>
update fix code t11
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_lien_cong_ty_ver2.0.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FW\odoo\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3924448-4B19-4F5B-93FA-62B4F2E26BBE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
@@ -21,12 +22,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -78,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -109,12 +110,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -138,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -193,13 +194,13 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>DELL</author>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0">
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -269,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="1" shapeId="0">
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -295,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="1" shapeId="0">
+    <comment ref="P1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -321,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0">
+    <comment ref="AE1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -348,7 +349,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="60">
   <si>
     <t>Note</t>
   </si>
@@ -1006,12 +1007,15 @@
   </si>
   <si>
     <t>Kho nguồn</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng / Mô tả</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
@@ -1543,59 +1547,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.42578125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="30.85546875" style="6" customWidth="1"/>
-    <col min="25" max="25" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="22.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="24.140625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="22.140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="23.140625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" style="1" customWidth="1"/>
-    <col min="38" max="38" width="25.85546875" style="1" customWidth="1"/>
-    <col min="39" max="39" width="20.140625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="22.5703125" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="8.85546875" style="1"/>
+    <col min="8" max="8" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="39.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.88671875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="32.44140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.88671875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="30.88671875" style="6" customWidth="1"/>
+    <col min="26" max="26" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.5546875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="24.109375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="22.109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="23.109375" style="1" customWidth="1"/>
+    <col min="38" max="38" width="14.109375" style="1" customWidth="1"/>
+    <col min="39" max="39" width="25.88671875" style="1" customWidth="1"/>
+    <col min="40" max="40" width="20.109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="22.5546875" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="15" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="15" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1639,61 +1644,64 @@
         <v>23</v>
       </c>
       <c r="O1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1736,59 +1744,59 @@
       <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="1" t="b">
+      <c r="P2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>20</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="12">
+      <c r="S2" s="12">
         <v>1</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>10</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>2</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="18" t="s">
+      <c r="Z2" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="1">
+      <c r="AA2" s="1">
         <v>1</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>23960</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>50</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <v>1198000</v>
       </c>
-      <c r="AF2" s="1" t="b">
+      <c r="AG2" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
   </sheetData>
@@ -1799,45 +1807,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="31.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" customWidth="1"/>
-    <col min="14" max="14" width="33.42578125" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" customWidth="1"/>
+    <col min="1" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
+    <col min="12" max="12" width="31.109375" customWidth="1"/>
+    <col min="13" max="13" width="26.33203125" customWidth="1"/>
+    <col min="14" max="14" width="33.44140625" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" customWidth="1"/>
     <col min="16" max="16" width="35" customWidth="1"/>
-    <col min="17" max="17" width="35.7109375" customWidth="1"/>
-    <col min="18" max="18" width="30.7109375" customWidth="1"/>
-    <col min="19" max="19" width="27.7109375" customWidth="1"/>
+    <col min="17" max="17" width="35.6640625" customWidth="1"/>
+    <col min="18" max="18" width="30.6640625" customWidth="1"/>
+    <col min="19" max="19" width="27.6640625" customWidth="1"/>
     <col min="20" max="20" width="27" customWidth="1"/>
-    <col min="21" max="21" width="27.85546875" customWidth="1"/>
-    <col min="22" max="22" width="29.140625" customWidth="1"/>
-    <col min="23" max="23" width="34.5703125" customWidth="1"/>
-    <col min="24" max="24" width="29.42578125" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" customWidth="1"/>
-    <col min="26" max="26" width="15.42578125" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" customWidth="1"/>
-    <col min="28" max="28" width="25.85546875" customWidth="1"/>
-    <col min="29" max="29" width="22.42578125" customWidth="1"/>
-    <col min="30" max="30" width="25.140625" customWidth="1"/>
+    <col min="21" max="21" width="27.88671875" customWidth="1"/>
+    <col min="22" max="22" width="29.109375" customWidth="1"/>
+    <col min="23" max="23" width="34.5546875" customWidth="1"/>
+    <col min="24" max="24" width="29.44140625" customWidth="1"/>
+    <col min="25" max="25" width="19.88671875" customWidth="1"/>
+    <col min="26" max="26" width="15.44140625" customWidth="1"/>
+    <col min="27" max="27" width="14.5546875" customWidth="1"/>
+    <col min="28" max="28" width="25.88671875" customWidth="1"/>
+    <col min="29" max="29" width="22.44140625" customWidth="1"/>
+    <col min="30" max="30" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1908,7 +1916,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1984,58 +1992,58 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="1" bestFit="1"/>
-    <col min="4" max="4" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1" bestFit="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="33.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="32.7109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="27.7109375" customWidth="1"/>
-    <col min="25" max="25" width="30.85546875" style="6" customWidth="1"/>
-    <col min="26" max="26" width="20.140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.6640625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="36.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.88671875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="27.6640625" customWidth="1"/>
+    <col min="25" max="25" width="30.88671875" style="6" customWidth="1"/>
+    <col min="26" max="26" width="20.109375" style="1" customWidth="1"/>
+    <col min="27" max="27" width="16.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="22.7109375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="24.28515625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="22.140625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="23.140625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="14.140625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="25.85546875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="20.140625" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.7109375" style="1" customWidth="1"/>
-    <col min="40" max="16384" width="8.85546875" style="1"/>
+    <col min="32" max="32" width="22.6640625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="24.33203125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="22.109375" style="1" customWidth="1"/>
+    <col min="35" max="35" width="23.109375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="14.109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="25.88671875" style="1" customWidth="1"/>
+    <col min="38" max="38" width="20.109375" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.6640625" style="1" customWidth="1"/>
+    <col min="40" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -2218,7 +2226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
   </sheetData>
@@ -2231,12 +2239,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2372,15 +2377,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6a70de89-a9ee-4e6f-a4d0-6241823bbbed"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2404,17 +2420,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6a70de89-a9ee-4e6f-a4d0-6241823bbbed"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>